<commit_message>
Handle Notification on a separate UART for the MOTOR_BOARD
</commit_message>
<xml_diff>
--- a/documentation/robotConfigDocumentation.xlsx
+++ b/documentation/robotConfigDocumentation.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\dev\git\cen-electronic\documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{ABF782A8-8B55-4D59-82E4-6FA90CF7F940}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{AA5889DC-C1F5-4DBC-87E4-3B56E9C5CCA6}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28770" windowHeight="12195" xr2:uid="{20076331-22D9-4B41-BA60-0AA01759602F}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="12">
   <si>
     <t>STRATEGY</t>
   </si>
@@ -51,13 +51,16 @@
     <t>GREEN</t>
   </si>
   <si>
-    <t>SONAR_ON</t>
-  </si>
-  <si>
     <t>LEFT SWITCH</t>
   </si>
   <si>
     <t>RIGHT SWITCH</t>
+  </si>
+  <si>
+    <t>SONAR FAR</t>
+  </si>
+  <si>
+    <t>SONAR_NEAR</t>
   </si>
 </sst>
 </file>
@@ -391,15 +394,6 @@
     <xf numFmtId="0" fontId="4" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -413,6 +407,15 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -729,10 +732,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BB30C74F-688B-4291-A288-BAE3AC05A486}">
-  <dimension ref="A1:P11"/>
+  <dimension ref="A1:P12"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="S12" sqref="S12"/>
+      <selection activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -744,69 +747,69 @@
   <sheetData>
     <row r="1" spans="1:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="4"/>
-      <c r="B1" s="32" t="s">
+      <c r="B1" s="37" t="s">
+        <v>8</v>
+      </c>
+      <c r="C1" s="38"/>
+      <c r="D1" s="38"/>
+      <c r="E1" s="38"/>
+      <c r="F1" s="38"/>
+      <c r="G1" s="39"/>
+      <c r="H1" s="2"/>
+      <c r="I1" s="37" t="s">
         <v>9</v>
       </c>
-      <c r="C1" s="33"/>
-      <c r="D1" s="33"/>
-      <c r="E1" s="33"/>
-      <c r="F1" s="33"/>
-      <c r="G1" s="34"/>
-      <c r="H1" s="2"/>
-      <c r="I1" s="32" t="s">
-        <v>10</v>
-      </c>
-      <c r="J1" s="33"/>
-      <c r="K1" s="33"/>
-      <c r="L1" s="33"/>
-      <c r="M1" s="33"/>
-      <c r="N1" s="33"/>
-      <c r="O1" s="33"/>
-      <c r="P1" s="34"/>
+      <c r="J1" s="38"/>
+      <c r="K1" s="38"/>
+      <c r="L1" s="38"/>
+      <c r="M1" s="38"/>
+      <c r="N1" s="38"/>
+      <c r="O1" s="38"/>
+      <c r="P1" s="39"/>
     </row>
     <row r="2" spans="1:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="5"/>
-      <c r="B2" s="35">
+      <c r="B2" s="32">
         <v>1</v>
       </c>
-      <c r="C2" s="36">
+      <c r="C2" s="33">
         <v>2</v>
       </c>
-      <c r="D2" s="36">
+      <c r="D2" s="33">
         <v>3</v>
       </c>
-      <c r="E2" s="37">
+      <c r="E2" s="34">
         <v>4</v>
       </c>
-      <c r="F2" s="36">
+      <c r="F2" s="33">
         <v>5</v>
       </c>
-      <c r="G2" s="38">
+      <c r="G2" s="35">
         <v>6</v>
       </c>
-      <c r="H2" s="39"/>
-      <c r="I2" s="35">
+      <c r="H2" s="36"/>
+      <c r="I2" s="32">
         <v>1</v>
       </c>
-      <c r="J2" s="36">
+      <c r="J2" s="33">
         <v>2</v>
       </c>
-      <c r="K2" s="36">
+      <c r="K2" s="33">
         <v>3</v>
       </c>
-      <c r="L2" s="36">
+      <c r="L2" s="33">
         <v>4</v>
       </c>
-      <c r="M2" s="36">
+      <c r="M2" s="33">
         <v>5</v>
       </c>
-      <c r="N2" s="36">
+      <c r="N2" s="33">
         <v>6</v>
       </c>
-      <c r="O2" s="36">
+      <c r="O2" s="33">
         <v>7</v>
       </c>
-      <c r="P2" s="38">
+      <c r="P2" s="35">
         <v>8</v>
       </c>
     </row>
@@ -875,132 +878,154 @@
       <c r="P5" s="20"/>
     </row>
     <row r="6" spans="1:16" ht="12" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="29" t="s">
-        <v>8</v>
-      </c>
-      <c r="B6" s="12"/>
-      <c r="C6" s="13"/>
-      <c r="D6" s="13"/>
-      <c r="E6" s="14"/>
-      <c r="F6" s="13"/>
-      <c r="G6" s="15"/>
+      <c r="A6" s="30" t="s">
+        <v>10</v>
+      </c>
+      <c r="B6" s="3"/>
+      <c r="C6" s="18"/>
+      <c r="D6" s="18"/>
+      <c r="E6" s="19"/>
+      <c r="F6" s="18"/>
+      <c r="G6" s="20"/>
       <c r="H6" s="16"/>
-      <c r="I6" s="12"/>
-      <c r="J6" s="13"/>
+      <c r="I6" s="3"/>
+      <c r="J6" s="18"/>
       <c r="K6" s="17" t="s">
         <v>2</v>
       </c>
-      <c r="L6" s="13"/>
-      <c r="M6" s="13"/>
-      <c r="N6" s="13"/>
-      <c r="O6" s="13"/>
-      <c r="P6" s="15"/>
+      <c r="L6" s="18"/>
+      <c r="M6" s="18"/>
+      <c r="N6" s="18"/>
+      <c r="O6" s="18"/>
+      <c r="P6" s="20"/>
     </row>
     <row r="7" spans="1:16" ht="12" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="30" t="s">
+      <c r="A7" s="29" t="s">
+        <v>11</v>
+      </c>
+      <c r="B7" s="12"/>
+      <c r="C7" s="13"/>
+      <c r="D7" s="13"/>
+      <c r="E7" s="14"/>
+      <c r="F7" s="13"/>
+      <c r="G7" s="15"/>
+      <c r="H7" s="16"/>
+      <c r="I7" s="12"/>
+      <c r="J7" s="17" t="s">
+        <v>2</v>
+      </c>
+      <c r="K7" s="13"/>
+      <c r="L7" s="13"/>
+      <c r="M7" s="13"/>
+      <c r="N7" s="13"/>
+      <c r="O7" s="13"/>
+      <c r="P7" s="15"/>
+    </row>
+    <row r="8" spans="1:16" ht="12" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="30" t="s">
         <v>7</v>
       </c>
-      <c r="B7" s="3"/>
-      <c r="C7" s="18"/>
-      <c r="D7" s="18"/>
-      <c r="E7" s="19"/>
-      <c r="F7" s="18"/>
-      <c r="G7" s="20"/>
-      <c r="H7" s="16"/>
-      <c r="I7" s="21" t="s">
+      <c r="B8" s="3"/>
+      <c r="C8" s="18"/>
+      <c r="D8" s="18"/>
+      <c r="E8" s="19"/>
+      <c r="F8" s="18"/>
+      <c r="G8" s="20"/>
+      <c r="H8" s="16"/>
+      <c r="I8" s="21" t="s">
         <v>2</v>
       </c>
-      <c r="J7" s="18"/>
-      <c r="K7" s="18"/>
-      <c r="L7" s="18"/>
-      <c r="M7" s="18"/>
-      <c r="N7" s="18"/>
-      <c r="O7" s="18"/>
-      <c r="P7" s="20"/>
-    </row>
-    <row r="8" spans="1:16" ht="12" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="29"/>
-      <c r="B8" s="12"/>
-      <c r="C8" s="13"/>
-      <c r="D8" s="13"/>
-      <c r="E8" s="14"/>
-      <c r="F8" s="13"/>
-      <c r="G8" s="15"/>
-      <c r="H8" s="16"/>
-      <c r="I8" s="12"/>
-      <c r="J8" s="13"/>
-      <c r="K8" s="13"/>
-      <c r="L8" s="13"/>
-      <c r="M8" s="13"/>
-      <c r="N8" s="13"/>
-      <c r="O8" s="13"/>
-      <c r="P8" s="15"/>
+      <c r="J8" s="18"/>
+      <c r="K8" s="18"/>
+      <c r="L8" s="18"/>
+      <c r="M8" s="18"/>
+      <c r="N8" s="18"/>
+      <c r="O8" s="18"/>
+      <c r="P8" s="20"/>
     </row>
     <row r="9" spans="1:16" ht="12" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="30" t="s">
+      <c r="A9" s="29"/>
+      <c r="B9" s="12"/>
+      <c r="C9" s="13"/>
+      <c r="D9" s="13"/>
+      <c r="E9" s="14"/>
+      <c r="F9" s="13"/>
+      <c r="G9" s="15"/>
+      <c r="H9" s="16"/>
+      <c r="I9" s="12"/>
+      <c r="J9" s="13"/>
+      <c r="K9" s="13"/>
+      <c r="L9" s="13"/>
+      <c r="M9" s="13"/>
+      <c r="N9" s="13"/>
+      <c r="O9" s="13"/>
+      <c r="P9" s="15"/>
+    </row>
+    <row r="10" spans="1:16" ht="12" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="30" t="s">
         <v>4</v>
       </c>
-      <c r="B9" s="3"/>
-      <c r="C9" s="18"/>
-      <c r="D9" s="18"/>
-      <c r="E9" s="19"/>
-      <c r="F9" s="18"/>
-      <c r="G9" s="22" t="s">
+      <c r="B10" s="3"/>
+      <c r="C10" s="18"/>
+      <c r="D10" s="18"/>
+      <c r="E10" s="19"/>
+      <c r="F10" s="18"/>
+      <c r="G10" s="22" t="s">
         <v>2</v>
       </c>
-      <c r="H9" s="16"/>
-      <c r="I9" s="3"/>
-      <c r="J9" s="18"/>
-      <c r="K9" s="18"/>
-      <c r="L9" s="18"/>
-      <c r="M9" s="18"/>
-      <c r="N9" s="18"/>
-      <c r="O9" s="18"/>
-      <c r="P9" s="20"/>
-    </row>
-    <row r="10" spans="1:16" ht="12" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="29" t="s">
+      <c r="H10" s="16"/>
+      <c r="I10" s="3"/>
+      <c r="J10" s="18"/>
+      <c r="K10" s="18"/>
+      <c r="L10" s="18"/>
+      <c r="M10" s="18"/>
+      <c r="N10" s="18"/>
+      <c r="O10" s="18"/>
+      <c r="P10" s="20"/>
+    </row>
+    <row r="11" spans="1:16" ht="12" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="29" t="s">
         <v>5</v>
       </c>
-      <c r="B10" s="12"/>
-      <c r="C10" s="13"/>
-      <c r="D10" s="13"/>
-      <c r="E10" s="14"/>
-      <c r="F10" s="17" t="s">
+      <c r="B11" s="12"/>
+      <c r="C11" s="13"/>
+      <c r="D11" s="13"/>
+      <c r="E11" s="14"/>
+      <c r="F11" s="17" t="s">
         <v>2</v>
       </c>
-      <c r="G10" s="15"/>
-      <c r="H10" s="16"/>
-      <c r="I10" s="12"/>
-      <c r="J10" s="13"/>
-      <c r="K10" s="13"/>
-      <c r="L10" s="13"/>
-      <c r="M10" s="13"/>
-      <c r="N10" s="13"/>
-      <c r="O10" s="13"/>
-      <c r="P10" s="15"/>
-    </row>
-    <row r="11" spans="1:16" ht="12" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="31" t="s">
+      <c r="G11" s="15"/>
+      <c r="H11" s="16"/>
+      <c r="I11" s="12"/>
+      <c r="J11" s="13"/>
+      <c r="K11" s="13"/>
+      <c r="L11" s="13"/>
+      <c r="M11" s="13"/>
+      <c r="N11" s="13"/>
+      <c r="O11" s="13"/>
+      <c r="P11" s="15"/>
+    </row>
+    <row r="12" spans="1:16" ht="12" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A12" s="31" t="s">
         <v>6</v>
       </c>
-      <c r="B11" s="23"/>
-      <c r="C11" s="24"/>
-      <c r="D11" s="24"/>
-      <c r="E11" s="25" t="s">
+      <c r="B12" s="23"/>
+      <c r="C12" s="24"/>
+      <c r="D12" s="24"/>
+      <c r="E12" s="25" t="s">
         <v>2</v>
       </c>
-      <c r="F11" s="24"/>
-      <c r="G11" s="26"/>
-      <c r="H11" s="27"/>
-      <c r="I11" s="23"/>
-      <c r="J11" s="24"/>
-      <c r="K11" s="24"/>
-      <c r="L11" s="24"/>
-      <c r="M11" s="24"/>
-      <c r="N11" s="24"/>
-      <c r="O11" s="24"/>
-      <c r="P11" s="26"/>
+      <c r="F12" s="24"/>
+      <c r="G12" s="26"/>
+      <c r="H12" s="27"/>
+      <c r="I12" s="23"/>
+      <c r="J12" s="24"/>
+      <c r="K12" s="24"/>
+      <c r="L12" s="24"/>
+      <c r="M12" s="24"/>
+      <c r="N12" s="24"/>
+      <c r="O12" s="24"/>
+      <c r="P12" s="26"/>
     </row>
   </sheetData>
   <mergeCells count="2">

</xml_diff>

<commit_message>
Fix tofList Debug, update the start Point for Big and Small robot, fix tof Index
</commit_message>
<xml_diff>
--- a/documentation/robotConfigDocumentation.xlsx
+++ b/documentation/robotConfigDocumentation.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="19226"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21425"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\dev\git\cen-electronic\documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{AA5889DC-C1F5-4DBC-87E4-3B56E9C5CCA6}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A59FD99B-1C37-4F2C-B64B-B9922877C9C0}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28770" windowHeight="12195" xr2:uid="{20076331-22D9-4B41-BA60-0AA01759602F}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{20076331-22D9-4B41-BA60-0AA01759602F}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="15">
   <si>
     <t>STRATEGY</t>
   </si>
@@ -48,9 +48,6 @@
     <t>ULTRA_LOW</t>
   </si>
   <si>
-    <t>GREEN</t>
-  </si>
-  <si>
     <t>LEFT SWITCH</t>
   </si>
   <si>
@@ -61,6 +58,18 @@
   </si>
   <si>
     <t>SONAR_NEAR</t>
+  </si>
+  <si>
+    <t>YELLOW</t>
+  </si>
+  <si>
+    <t>LCD</t>
+  </si>
+  <si>
+    <t>DEBUG</t>
+  </si>
+  <si>
+    <t>UNDEFINED</t>
   </si>
 </sst>
 </file>
@@ -130,7 +139,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="20">
+  <borders count="21">
     <border>
       <left/>
       <right/>
@@ -355,13 +364,22 @@
       <bottom style="medium">
         <color indexed="64"/>
       </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
       <diagonal/>
     </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="40">
+  <cellXfs count="51">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
@@ -383,17 +401,12 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -418,6 +431,28 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -732,10 +767,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BB30C74F-688B-4291-A288-BAE3AC05A486}">
-  <dimension ref="A1:P12"/>
+  <dimension ref="A1:P15"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="A7" sqref="A7"/>
+    <sheetView tabSelected="1" zoomScale="175" zoomScaleNormal="175" workbookViewId="0">
+      <selection activeCell="A14" sqref="A14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -747,74 +782,74 @@
   <sheetData>
     <row r="1" spans="1:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="4"/>
-      <c r="B1" s="37" t="s">
+      <c r="B1" s="32" t="s">
+        <v>7</v>
+      </c>
+      <c r="C1" s="33"/>
+      <c r="D1" s="33"/>
+      <c r="E1" s="33"/>
+      <c r="F1" s="33"/>
+      <c r="G1" s="34"/>
+      <c r="H1" s="2"/>
+      <c r="I1" s="32" t="s">
         <v>8</v>
       </c>
-      <c r="C1" s="38"/>
-      <c r="D1" s="38"/>
-      <c r="E1" s="38"/>
-      <c r="F1" s="38"/>
-      <c r="G1" s="39"/>
-      <c r="H1" s="2"/>
-      <c r="I1" s="37" t="s">
-        <v>9</v>
-      </c>
-      <c r="J1" s="38"/>
-      <c r="K1" s="38"/>
-      <c r="L1" s="38"/>
-      <c r="M1" s="38"/>
-      <c r="N1" s="38"/>
-      <c r="O1" s="38"/>
-      <c r="P1" s="39"/>
+      <c r="J1" s="33"/>
+      <c r="K1" s="33"/>
+      <c r="L1" s="33"/>
+      <c r="M1" s="33"/>
+      <c r="N1" s="33"/>
+      <c r="O1" s="33"/>
+      <c r="P1" s="34"/>
     </row>
     <row r="2" spans="1:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="5"/>
-      <c r="B2" s="32">
+      <c r="B2" s="27">
         <v>1</v>
       </c>
-      <c r="C2" s="33">
-        <v>2</v>
-      </c>
-      <c r="D2" s="33">
+      <c r="C2" s="28">
+        <v>2</v>
+      </c>
+      <c r="D2" s="28">
         <v>3</v>
       </c>
-      <c r="E2" s="34">
+      <c r="E2" s="29">
         <v>4</v>
       </c>
-      <c r="F2" s="33">
+      <c r="F2" s="28">
         <v>5</v>
       </c>
-      <c r="G2" s="35">
+      <c r="G2" s="30">
         <v>6</v>
       </c>
-      <c r="H2" s="36"/>
-      <c r="I2" s="32">
+      <c r="H2" s="31"/>
+      <c r="I2" s="27">
         <v>1</v>
       </c>
-      <c r="J2" s="33">
-        <v>2</v>
-      </c>
-      <c r="K2" s="33">
+      <c r="J2" s="28">
+        <v>2</v>
+      </c>
+      <c r="K2" s="28">
         <v>3</v>
       </c>
-      <c r="L2" s="33">
+      <c r="L2" s="28">
         <v>4</v>
       </c>
-      <c r="M2" s="33">
+      <c r="M2" s="28">
         <v>5</v>
       </c>
-      <c r="N2" s="33">
+      <c r="N2" s="28">
         <v>6</v>
       </c>
-      <c r="O2" s="33">
+      <c r="O2" s="28">
         <v>7</v>
       </c>
-      <c r="P2" s="35">
+      <c r="P2" s="30">
         <v>8</v>
       </c>
     </row>
     <row r="3" spans="1:16" ht="12" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="28" t="s">
+      <c r="A3" s="24" t="s">
         <v>0</v>
       </c>
       <c r="B3" s="1"/>
@@ -834,7 +869,7 @@
       <c r="P3" s="11"/>
     </row>
     <row r="4" spans="1:16" ht="12" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="29" t="s">
+      <c r="A4" s="25" t="s">
         <v>1</v>
       </c>
       <c r="B4" s="12"/>
@@ -856,7 +891,7 @@
       <c r="P4" s="15"/>
     </row>
     <row r="5" spans="1:16" ht="12" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="30" t="s">
+      <c r="A5" s="26" t="s">
         <v>3</v>
       </c>
       <c r="B5" s="3"/>
@@ -878,113 +913,113 @@
       <c r="P5" s="20"/>
     </row>
     <row r="6" spans="1:16" ht="12" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="30" t="s">
-        <v>10</v>
-      </c>
-      <c r="B6" s="3"/>
-      <c r="C6" s="18"/>
-      <c r="D6" s="18"/>
-      <c r="E6" s="19"/>
-      <c r="F6" s="18"/>
-      <c r="G6" s="20"/>
+      <c r="A6" s="25" t="s">
+        <v>9</v>
+      </c>
+      <c r="B6" s="12"/>
+      <c r="C6" s="13"/>
+      <c r="D6" s="13"/>
+      <c r="E6" s="14"/>
+      <c r="F6" s="13"/>
+      <c r="G6" s="15"/>
       <c r="H6" s="16"/>
-      <c r="I6" s="3"/>
+      <c r="I6" s="12"/>
       <c r="J6" s="18"/>
       <c r="K6" s="17" t="s">
         <v>2</v>
       </c>
-      <c r="L6" s="18"/>
-      <c r="M6" s="18"/>
-      <c r="N6" s="18"/>
-      <c r="O6" s="18"/>
-      <c r="P6" s="20"/>
+      <c r="L6" s="13"/>
+      <c r="M6" s="13"/>
+      <c r="N6" s="13"/>
+      <c r="O6" s="13"/>
+      <c r="P6" s="15"/>
     </row>
     <row r="7" spans="1:16" ht="12" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="29" t="s">
+      <c r="A7" s="26" t="s">
+        <v>10</v>
+      </c>
+      <c r="B7" s="3"/>
+      <c r="C7" s="18"/>
+      <c r="D7" s="18"/>
+      <c r="E7" s="19"/>
+      <c r="F7" s="18"/>
+      <c r="G7" s="20"/>
+      <c r="H7" s="16"/>
+      <c r="I7" s="39"/>
+      <c r="J7" s="17" t="s">
+        <v>2</v>
+      </c>
+      <c r="K7" s="18"/>
+      <c r="L7" s="18"/>
+      <c r="M7" s="18"/>
+      <c r="N7" s="18"/>
+      <c r="O7" s="18"/>
+      <c r="P7" s="20"/>
+    </row>
+    <row r="8" spans="1:16" ht="12" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A8" s="45" t="s">
         <v>11</v>
       </c>
-      <c r="B7" s="12"/>
-      <c r="C7" s="13"/>
-      <c r="D7" s="13"/>
-      <c r="E7" s="14"/>
-      <c r="F7" s="13"/>
-      <c r="G7" s="15"/>
-      <c r="H7" s="16"/>
-      <c r="I7" s="12"/>
-      <c r="J7" s="17" t="s">
-        <v>2</v>
-      </c>
-      <c r="K7" s="13"/>
-      <c r="L7" s="13"/>
-      <c r="M7" s="13"/>
-      <c r="N7" s="13"/>
-      <c r="O7" s="13"/>
-      <c r="P7" s="15"/>
-    </row>
-    <row r="8" spans="1:16" ht="12" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="30" t="s">
-        <v>7</v>
-      </c>
-      <c r="B8" s="3"/>
-      <c r="C8" s="18"/>
-      <c r="D8" s="18"/>
-      <c r="E8" s="19"/>
-      <c r="F8" s="18"/>
-      <c r="G8" s="20"/>
-      <c r="H8" s="16"/>
-      <c r="I8" s="21" t="s">
-        <v>2</v>
-      </c>
-      <c r="J8" s="18"/>
-      <c r="K8" s="18"/>
-      <c r="L8" s="18"/>
-      <c r="M8" s="18"/>
-      <c r="N8" s="18"/>
-      <c r="O8" s="18"/>
-      <c r="P8" s="20"/>
-    </row>
-    <row r="9" spans="1:16" ht="12" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="29"/>
-      <c r="B9" s="12"/>
-      <c r="C9" s="13"/>
-      <c r="D9" s="13"/>
-      <c r="E9" s="14"/>
-      <c r="F9" s="13"/>
-      <c r="G9" s="15"/>
-      <c r="H9" s="16"/>
-      <c r="I9" s="12"/>
-      <c r="J9" s="13"/>
-      <c r="K9" s="13"/>
-      <c r="L9" s="13"/>
-      <c r="M9" s="13"/>
-      <c r="N9" s="13"/>
-      <c r="O9" s="13"/>
-      <c r="P9" s="15"/>
+      <c r="B8" s="40"/>
+      <c r="C8" s="41"/>
+      <c r="D8" s="41"/>
+      <c r="E8" s="42"/>
+      <c r="F8" s="41"/>
+      <c r="G8" s="43"/>
+      <c r="H8" s="23"/>
+      <c r="I8" s="44" t="s">
+        <v>2</v>
+      </c>
+      <c r="J8" s="21"/>
+      <c r="K8" s="21"/>
+      <c r="L8" s="21"/>
+      <c r="M8" s="21"/>
+      <c r="N8" s="21"/>
+      <c r="O8" s="21"/>
+      <c r="P8" s="22"/>
+    </row>
+    <row r="9" spans="1:16" ht="9" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A9" s="35"/>
+      <c r="B9" s="36"/>
+      <c r="C9" s="36"/>
+      <c r="D9" s="36"/>
+      <c r="E9" s="36"/>
+      <c r="F9" s="36"/>
+      <c r="G9" s="36"/>
+      <c r="H9" s="36"/>
+      <c r="I9" s="36"/>
+      <c r="J9" s="36"/>
+      <c r="K9" s="36"/>
+      <c r="L9" s="36"/>
+      <c r="M9" s="36"/>
+      <c r="N9" s="36"/>
+      <c r="O9" s="36"/>
+      <c r="P9" s="37"/>
     </row>
     <row r="10" spans="1:16" ht="12" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="30" t="s">
+      <c r="A10" s="24" t="s">
         <v>4</v>
       </c>
-      <c r="B10" s="3"/>
-      <c r="C10" s="18"/>
-      <c r="D10" s="18"/>
-      <c r="E10" s="19"/>
-      <c r="F10" s="18"/>
-      <c r="G10" s="22" t="s">
-        <v>2</v>
-      </c>
-      <c r="H10" s="16"/>
-      <c r="I10" s="3"/>
-      <c r="J10" s="18"/>
-      <c r="K10" s="18"/>
-      <c r="L10" s="18"/>
-      <c r="M10" s="18"/>
-      <c r="N10" s="18"/>
-      <c r="O10" s="18"/>
-      <c r="P10" s="20"/>
+      <c r="B10" s="1"/>
+      <c r="C10" s="6"/>
+      <c r="D10" s="6"/>
+      <c r="E10" s="7"/>
+      <c r="F10" s="6"/>
+      <c r="G10" s="11" t="s">
+        <v>2</v>
+      </c>
+      <c r="H10" s="9"/>
+      <c r="I10" s="1"/>
+      <c r="J10" s="6"/>
+      <c r="K10" s="6"/>
+      <c r="L10" s="6"/>
+      <c r="M10" s="6"/>
+      <c r="N10" s="6"/>
+      <c r="O10" s="6"/>
+      <c r="P10" s="8"/>
     </row>
     <row r="11" spans="1:16" ht="12" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="29" t="s">
+      <c r="A11" s="25" t="s">
         <v>5</v>
       </c>
       <c r="B11" s="12"/>
@@ -1005,32 +1040,99 @@
       <c r="O11" s="13"/>
       <c r="P11" s="15"/>
     </row>
-    <row r="12" spans="1:16" ht="12" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="31" t="s">
+    <row r="12" spans="1:16" ht="12" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="46" t="s">
         <v>6</v>
       </c>
-      <c r="B12" s="23"/>
-      <c r="C12" s="24"/>
-      <c r="D12" s="24"/>
-      <c r="E12" s="25" t="s">
-        <v>2</v>
-      </c>
-      <c r="F12" s="24"/>
-      <c r="G12" s="26"/>
-      <c r="H12" s="27"/>
-      <c r="I12" s="23"/>
-      <c r="J12" s="24"/>
-      <c r="K12" s="24"/>
-      <c r="L12" s="24"/>
-      <c r="M12" s="24"/>
-      <c r="N12" s="24"/>
-      <c r="O12" s="24"/>
-      <c r="P12" s="26"/>
+      <c r="B12" s="47"/>
+      <c r="C12" s="48"/>
+      <c r="D12" s="48"/>
+      <c r="E12" s="17" t="s">
+        <v>2</v>
+      </c>
+      <c r="F12" s="48"/>
+      <c r="G12" s="49"/>
+      <c r="H12" s="16"/>
+      <c r="I12" s="47"/>
+      <c r="J12" s="48"/>
+      <c r="K12" s="48"/>
+      <c r="L12" s="48"/>
+      <c r="M12" s="48"/>
+      <c r="N12" s="48"/>
+      <c r="O12" s="48"/>
+      <c r="P12" s="49"/>
+    </row>
+    <row r="13" spans="1:16" ht="12" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="25" t="s">
+        <v>14</v>
+      </c>
+      <c r="B13" s="12"/>
+      <c r="C13" s="13"/>
+      <c r="D13" s="17" t="s">
+        <v>2</v>
+      </c>
+      <c r="E13" s="14"/>
+      <c r="F13" s="14"/>
+      <c r="G13" s="15"/>
+      <c r="H13" s="16"/>
+      <c r="I13" s="12"/>
+      <c r="J13" s="13"/>
+      <c r="K13" s="13"/>
+      <c r="L13" s="13"/>
+      <c r="M13" s="13"/>
+      <c r="N13" s="13"/>
+      <c r="O13" s="13"/>
+      <c r="P13" s="15"/>
+    </row>
+    <row r="14" spans="1:16" ht="12" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A14" s="46" t="s">
+        <v>13</v>
+      </c>
+      <c r="B14" s="47"/>
+      <c r="C14" s="17" t="s">
+        <v>2</v>
+      </c>
+      <c r="D14" s="48"/>
+      <c r="E14" s="50"/>
+      <c r="F14" s="50"/>
+      <c r="G14" s="49"/>
+      <c r="H14" s="16"/>
+      <c r="I14" s="47"/>
+      <c r="J14" s="48"/>
+      <c r="K14" s="48"/>
+      <c r="L14" s="48"/>
+      <c r="M14" s="48"/>
+      <c r="N14" s="48"/>
+      <c r="O14" s="48"/>
+      <c r="P14" s="49"/>
+    </row>
+    <row r="15" spans="1:16" ht="12" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A15" s="45" t="s">
+        <v>12</v>
+      </c>
+      <c r="B15" s="38" t="s">
+        <v>2</v>
+      </c>
+      <c r="C15" s="41"/>
+      <c r="D15" s="41"/>
+      <c r="E15" s="41"/>
+      <c r="F15" s="41"/>
+      <c r="G15" s="43"/>
+      <c r="H15" s="23"/>
+      <c r="I15" s="40"/>
+      <c r="J15" s="41"/>
+      <c r="K15" s="41"/>
+      <c r="L15" s="41"/>
+      <c r="M15" s="41"/>
+      <c r="N15" s="41"/>
+      <c r="O15" s="41"/>
+      <c r="P15" s="43"/>
     </row>
   </sheetData>
-  <mergeCells count="2">
+  <mergeCells count="3">
     <mergeCell ref="B1:G1"/>
     <mergeCell ref="I1:P1"/>
+    <mergeCell ref="A9:P9"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>

</xml_diff>

<commit_message>
Refactor motionConstants to be able to have more Option on Speed, refactor robotConfig
</commit_message>
<xml_diff>
--- a/documentation/robotConfigDocumentation.xlsx
+++ b/documentation/robotConfigDocumentation.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\dev\git\cen-electronic\documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A59FD99B-1C37-4F2C-B64B-B9922877C9C0}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E50B7D8E-6062-4202-8CF9-C7263C8D39A1}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{20076331-22D9-4B41-BA60-0AA01759602F}"/>
+    <workbookView xWindow="12900" yWindow="2070" windowWidth="15510" windowHeight="11820" xr2:uid="{20076331-22D9-4B41-BA60-0AA01759602F}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,41 +25,20 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="12">
   <si>
     <t>STRATEGY</t>
   </si>
   <si>
-    <t>NO_WAIT_START</t>
-  </si>
-  <si>
     <t>C</t>
   </si>
   <si>
-    <t>NO_END</t>
-  </si>
-  <si>
-    <t>LOW</t>
-  </si>
-  <si>
-    <t>VERY_LOW</t>
-  </si>
-  <si>
-    <t>ULTRA_LOW</t>
-  </si>
-  <si>
     <t>LEFT SWITCH</t>
   </si>
   <si>
     <t>RIGHT SWITCH</t>
   </si>
   <si>
-    <t>SONAR FAR</t>
-  </si>
-  <si>
-    <t>SONAR_NEAR</t>
-  </si>
-  <si>
     <t>YELLOW</t>
   </si>
   <si>
@@ -69,7 +48,19 @@
     <t>DEBUG</t>
   </si>
   <si>
-    <t>UNDEFINED</t>
+    <t>SPEED</t>
+  </si>
+  <si>
+    <t>DON’T_WAIT_ST</t>
+  </si>
+  <si>
+    <t>DO_NOT_END</t>
+  </si>
+  <si>
+    <t>SONAR</t>
+  </si>
+  <si>
+    <t>STRAT_MANUAL</t>
   </si>
 </sst>
 </file>
@@ -139,7 +130,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="21">
+  <borders count="22">
     <border>
       <left/>
       <right/>
@@ -373,13 +364,22 @@
       </right>
       <top/>
       <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
       <diagonal/>
     </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="51">
+  <cellXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
@@ -422,6 +422,14 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -440,19 +448,9 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -767,10 +765,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BB30C74F-688B-4291-A288-BAE3AC05A486}">
-  <dimension ref="A1:P15"/>
+  <dimension ref="A1:P12"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="175" zoomScaleNormal="175" workbookViewId="0">
-      <selection activeCell="A14" sqref="A14"/>
+      <selection activeCell="E10" sqref="E10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -782,25 +780,25 @@
   <sheetData>
     <row r="1" spans="1:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="4"/>
-      <c r="B1" s="32" t="s">
-        <v>7</v>
-      </c>
-      <c r="C1" s="33"/>
-      <c r="D1" s="33"/>
-      <c r="E1" s="33"/>
-      <c r="F1" s="33"/>
-      <c r="G1" s="34"/>
+      <c r="B1" s="40" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1" s="41"/>
+      <c r="D1" s="41"/>
+      <c r="E1" s="41"/>
+      <c r="F1" s="41"/>
+      <c r="G1" s="42"/>
       <c r="H1" s="2"/>
-      <c r="I1" s="32" t="s">
-        <v>8</v>
-      </c>
-      <c r="J1" s="33"/>
-      <c r="K1" s="33"/>
-      <c r="L1" s="33"/>
-      <c r="M1" s="33"/>
-      <c r="N1" s="33"/>
-      <c r="O1" s="33"/>
-      <c r="P1" s="34"/>
+      <c r="I1" s="40" t="s">
+        <v>3</v>
+      </c>
+      <c r="J1" s="41"/>
+      <c r="K1" s="41"/>
+      <c r="L1" s="41"/>
+      <c r="M1" s="41"/>
+      <c r="N1" s="41"/>
+      <c r="O1" s="41"/>
+      <c r="P1" s="42"/>
     </row>
     <row r="2" spans="1:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="5"/>
@@ -870,7 +868,7 @@
     </row>
     <row r="4" spans="1:16" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="25" t="s">
-        <v>1</v>
+        <v>11</v>
       </c>
       <c r="B4" s="12"/>
       <c r="C4" s="13"/>
@@ -884,7 +882,7 @@
       <c r="K4" s="13"/>
       <c r="L4" s="13"/>
       <c r="M4" s="17" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="N4" s="13"/>
       <c r="O4" s="13"/>
@@ -892,7 +890,7 @@
     </row>
     <row r="5" spans="1:16" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="26" t="s">
-        <v>3</v>
+        <v>8</v>
       </c>
       <c r="B5" s="3"/>
       <c r="C5" s="18"/>
@@ -905,7 +903,7 @@
       <c r="J5" s="18"/>
       <c r="K5" s="18"/>
       <c r="L5" s="17" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="M5" s="18"/>
       <c r="N5" s="18"/>
@@ -926,7 +924,7 @@
       <c r="I6" s="12"/>
       <c r="J6" s="18"/>
       <c r="K6" s="17" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="L6" s="13"/>
       <c r="M6" s="13"/>
@@ -936,7 +934,7 @@
     </row>
     <row r="7" spans="1:16" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="26" t="s">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="B7" s="3"/>
       <c r="C7" s="18"/>
@@ -945,9 +943,9 @@
       <c r="F7" s="18"/>
       <c r="G7" s="20"/>
       <c r="H7" s="16"/>
-      <c r="I7" s="39"/>
+      <c r="I7" s="33"/>
       <c r="J7" s="17" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="K7" s="18"/>
       <c r="L7" s="18"/>
@@ -957,18 +955,18 @@
       <c r="P7" s="20"/>
     </row>
     <row r="8" spans="1:16" ht="12" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="45" t="s">
-        <v>11</v>
-      </c>
-      <c r="B8" s="40"/>
-      <c r="C8" s="41"/>
-      <c r="D8" s="41"/>
-      <c r="E8" s="42"/>
-      <c r="F8" s="41"/>
-      <c r="G8" s="43"/>
+      <c r="A8" s="39" t="s">
+        <v>4</v>
+      </c>
+      <c r="B8" s="34"/>
+      <c r="C8" s="35"/>
+      <c r="D8" s="35"/>
+      <c r="E8" s="36"/>
+      <c r="F8" s="35"/>
+      <c r="G8" s="37"/>
       <c r="H8" s="23"/>
-      <c r="I8" s="44" t="s">
-        <v>2</v>
+      <c r="I8" s="38" t="s">
+        <v>1</v>
       </c>
       <c r="J8" s="21"/>
       <c r="K8" s="21"/>
@@ -979,34 +977,38 @@
       <c r="P8" s="22"/>
     </row>
     <row r="9" spans="1:16" ht="9" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="35"/>
-      <c r="B9" s="36"/>
-      <c r="C9" s="36"/>
-      <c r="D9" s="36"/>
-      <c r="E9" s="36"/>
-      <c r="F9" s="36"/>
-      <c r="G9" s="36"/>
-      <c r="H9" s="36"/>
-      <c r="I9" s="36"/>
-      <c r="J9" s="36"/>
-      <c r="K9" s="36"/>
-      <c r="L9" s="36"/>
-      <c r="M9" s="36"/>
-      <c r="N9" s="36"/>
-      <c r="O9" s="36"/>
-      <c r="P9" s="37"/>
+      <c r="A9" s="43"/>
+      <c r="B9" s="44"/>
+      <c r="C9" s="44"/>
+      <c r="D9" s="44"/>
+      <c r="E9" s="44"/>
+      <c r="F9" s="44"/>
+      <c r="G9" s="44"/>
+      <c r="H9" s="44"/>
+      <c r="I9" s="44"/>
+      <c r="J9" s="44"/>
+      <c r="K9" s="44"/>
+      <c r="L9" s="44"/>
+      <c r="M9" s="44"/>
+      <c r="N9" s="44"/>
+      <c r="O9" s="44"/>
+      <c r="P9" s="45"/>
     </row>
     <row r="10" spans="1:16" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="24" t="s">
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="B10" s="1"/>
       <c r="C10" s="6"/>
       <c r="D10" s="6"/>
-      <c r="E10" s="7"/>
-      <c r="F10" s="6"/>
+      <c r="E10" s="10" t="s">
+        <v>1</v>
+      </c>
+      <c r="F10" s="10" t="s">
+        <v>1</v>
+      </c>
       <c r="G10" s="11" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="H10" s="9"/>
       <c r="I10" s="1"/>
@@ -1020,15 +1022,17 @@
     </row>
     <row r="11" spans="1:16" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="25" t="s">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="B11" s="12"/>
-      <c r="C11" s="13"/>
-      <c r="D11" s="13"/>
+      <c r="C11" s="17" t="s">
+        <v>1</v>
+      </c>
+      <c r="D11" s="17" t="s">
+        <v>1</v>
+      </c>
       <c r="E11" s="14"/>
-      <c r="F11" s="17" t="s">
-        <v>2</v>
-      </c>
+      <c r="F11" s="14"/>
       <c r="G11" s="15"/>
       <c r="H11" s="16"/>
       <c r="I11" s="12"/>
@@ -1040,93 +1044,25 @@
       <c r="O11" s="13"/>
       <c r="P11" s="15"/>
     </row>
-    <row r="12" spans="1:16" ht="12" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:16" ht="12" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A12" s="46" t="s">
-        <v>6</v>
-      </c>
-      <c r="B12" s="47"/>
-      <c r="C12" s="48"/>
-      <c r="D12" s="48"/>
-      <c r="E12" s="17" t="s">
-        <v>2</v>
-      </c>
-      <c r="F12" s="48"/>
-      <c r="G12" s="49"/>
-      <c r="H12" s="16"/>
-      <c r="I12" s="47"/>
+        <v>5</v>
+      </c>
+      <c r="B12" s="32"/>
+      <c r="C12" s="21"/>
+      <c r="D12" s="21"/>
+      <c r="E12" s="47"/>
+      <c r="F12" s="21"/>
+      <c r="G12" s="22"/>
+      <c r="H12" s="23"/>
+      <c r="I12" s="48"/>
       <c r="J12" s="48"/>
-      <c r="K12" s="48"/>
-      <c r="L12" s="48"/>
-      <c r="M12" s="48"/>
-      <c r="N12" s="48"/>
-      <c r="O12" s="48"/>
-      <c r="P12" s="49"/>
-    </row>
-    <row r="13" spans="1:16" ht="12" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="25" t="s">
-        <v>14</v>
-      </c>
-      <c r="B13" s="12"/>
-      <c r="C13" s="13"/>
-      <c r="D13" s="17" t="s">
-        <v>2</v>
-      </c>
-      <c r="E13" s="14"/>
-      <c r="F13" s="14"/>
-      <c r="G13" s="15"/>
-      <c r="H13" s="16"/>
-      <c r="I13" s="12"/>
-      <c r="J13" s="13"/>
-      <c r="K13" s="13"/>
-      <c r="L13" s="13"/>
-      <c r="M13" s="13"/>
-      <c r="N13" s="13"/>
-      <c r="O13" s="13"/>
-      <c r="P13" s="15"/>
-    </row>
-    <row r="14" spans="1:16" ht="12" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="46" t="s">
-        <v>13</v>
-      </c>
-      <c r="B14" s="47"/>
-      <c r="C14" s="17" t="s">
-        <v>2</v>
-      </c>
-      <c r="D14" s="48"/>
-      <c r="E14" s="50"/>
-      <c r="F14" s="50"/>
-      <c r="G14" s="49"/>
-      <c r="H14" s="16"/>
-      <c r="I14" s="47"/>
-      <c r="J14" s="48"/>
-      <c r="K14" s="48"/>
-      <c r="L14" s="48"/>
-      <c r="M14" s="48"/>
-      <c r="N14" s="48"/>
-      <c r="O14" s="48"/>
-      <c r="P14" s="49"/>
-    </row>
-    <row r="15" spans="1:16" ht="12" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="45" t="s">
-        <v>12</v>
-      </c>
-      <c r="B15" s="38" t="s">
-        <v>2</v>
-      </c>
-      <c r="C15" s="41"/>
-      <c r="D15" s="41"/>
-      <c r="E15" s="41"/>
-      <c r="F15" s="41"/>
-      <c r="G15" s="43"/>
-      <c r="H15" s="23"/>
-      <c r="I15" s="40"/>
-      <c r="J15" s="41"/>
-      <c r="K15" s="41"/>
-      <c r="L15" s="41"/>
-      <c r="M15" s="41"/>
-      <c r="N15" s="41"/>
-      <c r="O15" s="41"/>
-      <c r="P15" s="43"/>
+      <c r="K12" s="21"/>
+      <c r="L12" s="21"/>
+      <c r="M12" s="21"/>
+      <c r="N12" s="21"/>
+      <c r="O12" s="21"/>
+      <c r="P12" s="22"/>
     </row>
   </sheetData>
   <mergeCells count="3">

</xml_diff>

<commit_message>
Add Experience2019 Device to be able to debug more easily, protection agains bad value from tof. (NOT TESTED)
</commit_message>
<xml_diff>
--- a/documentation/robotConfigDocumentation.xlsx
+++ b/documentation/robotConfigDocumentation.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21425"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21601"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\dev\git\cen-electronic\documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E50B7D8E-6062-4202-8CF9-C7263C8D39A1}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5C35B7B6-BB46-4F76-9BCE-73AE9443A6B6}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="12900" yWindow="2070" windowWidth="15510" windowHeight="11820" xr2:uid="{20076331-22D9-4B41-BA60-0AA01759602F}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{20076331-22D9-4B41-BA60-0AA01759602F}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="12">
   <si>
     <t>STRATEGY</t>
   </si>
@@ -130,7 +130,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="22">
+  <borders count="23">
     <border>
       <left/>
       <right/>
@@ -375,11 +375,22 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="49">
+  <cellXfs count="53">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
@@ -423,13 +434,15 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -448,9 +461,13 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -765,10 +782,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BB30C74F-688B-4291-A288-BAE3AC05A486}">
-  <dimension ref="A1:P12"/>
+  <dimension ref="A1:P25"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="175" zoomScaleNormal="175" workbookViewId="0">
-      <selection activeCell="E10" sqref="E10"/>
+    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="D19" sqref="D19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -780,25 +797,25 @@
   <sheetData>
     <row r="1" spans="1:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="4"/>
-      <c r="B1" s="40" t="s">
+      <c r="B1" s="42" t="s">
         <v>2</v>
       </c>
-      <c r="C1" s="41"/>
-      <c r="D1" s="41"/>
-      <c r="E1" s="41"/>
-      <c r="F1" s="41"/>
-      <c r="G1" s="42"/>
+      <c r="C1" s="43"/>
+      <c r="D1" s="43"/>
+      <c r="E1" s="43"/>
+      <c r="F1" s="43"/>
+      <c r="G1" s="44"/>
       <c r="H1" s="2"/>
-      <c r="I1" s="40" t="s">
+      <c r="I1" s="42" t="s">
         <v>3</v>
       </c>
-      <c r="J1" s="41"/>
-      <c r="K1" s="41"/>
-      <c r="L1" s="41"/>
-      <c r="M1" s="41"/>
-      <c r="N1" s="41"/>
-      <c r="O1" s="41"/>
-      <c r="P1" s="42"/>
+      <c r="J1" s="43"/>
+      <c r="K1" s="43"/>
+      <c r="L1" s="43"/>
+      <c r="M1" s="43"/>
+      <c r="N1" s="43"/>
+      <c r="O1" s="43"/>
+      <c r="P1" s="44"/>
     </row>
     <row r="2" spans="1:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="5"/>
@@ -839,10 +856,10 @@
       <c r="N2" s="28">
         <v>6</v>
       </c>
-      <c r="O2" s="28">
+      <c r="O2" s="30">
         <v>7</v>
       </c>
-      <c r="P2" s="30">
+      <c r="P2" s="48">
         <v>8</v>
       </c>
     </row>
@@ -863,8 +880,8 @@
       <c r="L3" s="6"/>
       <c r="M3" s="6"/>
       <c r="N3" s="10"/>
-      <c r="O3" s="10"/>
-      <c r="P3" s="11"/>
+      <c r="O3" s="11"/>
+      <c r="P3" s="49"/>
     </row>
     <row r="4" spans="1:16" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="25" t="s">
@@ -885,8 +902,8 @@
         <v>1</v>
       </c>
       <c r="N4" s="13"/>
-      <c r="O4" s="13"/>
-      <c r="P4" s="15"/>
+      <c r="O4" s="15"/>
+      <c r="P4" s="50"/>
     </row>
     <row r="5" spans="1:16" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="26" t="s">
@@ -907,8 +924,8 @@
       </c>
       <c r="M5" s="18"/>
       <c r="N5" s="18"/>
-      <c r="O5" s="18"/>
-      <c r="P5" s="20"/>
+      <c r="O5" s="20"/>
+      <c r="P5" s="51"/>
     </row>
     <row r="6" spans="1:16" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="25" t="s">
@@ -922,15 +939,15 @@
       <c r="G6" s="15"/>
       <c r="H6" s="16"/>
       <c r="I6" s="12"/>
-      <c r="J6" s="18"/>
+      <c r="J6" s="13"/>
       <c r="K6" s="17" t="s">
         <v>1</v>
       </c>
       <c r="L6" s="13"/>
       <c r="M6" s="13"/>
       <c r="N6" s="13"/>
-      <c r="O6" s="13"/>
-      <c r="P6" s="15"/>
+      <c r="O6" s="15"/>
+      <c r="P6" s="50"/>
     </row>
     <row r="7" spans="1:16" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="26" t="s">
@@ -943,7 +960,7 @@
       <c r="F7" s="18"/>
       <c r="G7" s="20"/>
       <c r="H7" s="16"/>
-      <c r="I7" s="33"/>
+      <c r="I7" s="52"/>
       <c r="J7" s="17" t="s">
         <v>1</v>
       </c>
@@ -951,48 +968,48 @@
       <c r="L7" s="18"/>
       <c r="M7" s="18"/>
       <c r="N7" s="18"/>
-      <c r="O7" s="18"/>
-      <c r="P7" s="20"/>
+      <c r="O7" s="20"/>
+      <c r="P7" s="51"/>
     </row>
     <row r="8" spans="1:16" ht="12" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="39" t="s">
+      <c r="A8" s="38" t="s">
         <v>4</v>
       </c>
-      <c r="B8" s="34"/>
-      <c r="C8" s="35"/>
-      <c r="D8" s="35"/>
-      <c r="E8" s="36"/>
-      <c r="F8" s="35"/>
-      <c r="G8" s="37"/>
+      <c r="B8" s="33"/>
+      <c r="C8" s="34"/>
+      <c r="D8" s="34"/>
+      <c r="E8" s="35"/>
+      <c r="F8" s="34"/>
+      <c r="G8" s="36"/>
       <c r="H8" s="23"/>
-      <c r="I8" s="38" t="s">
-        <v>1</v>
-      </c>
-      <c r="J8" s="21"/>
-      <c r="K8" s="21"/>
-      <c r="L8" s="21"/>
-      <c r="M8" s="21"/>
-      <c r="N8" s="21"/>
-      <c r="O8" s="21"/>
-      <c r="P8" s="22"/>
+      <c r="I8" s="37" t="s">
+        <v>1</v>
+      </c>
+      <c r="J8" s="34"/>
+      <c r="K8" s="34"/>
+      <c r="L8" s="34"/>
+      <c r="M8" s="34"/>
+      <c r="N8" s="34"/>
+      <c r="O8" s="36"/>
+      <c r="P8" s="50"/>
     </row>
     <row r="9" spans="1:16" ht="9" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="43"/>
-      <c r="B9" s="44"/>
-      <c r="C9" s="44"/>
-      <c r="D9" s="44"/>
-      <c r="E9" s="44"/>
-      <c r="F9" s="44"/>
-      <c r="G9" s="44"/>
-      <c r="H9" s="44"/>
-      <c r="I9" s="44"/>
-      <c r="J9" s="44"/>
-      <c r="K9" s="44"/>
-      <c r="L9" s="44"/>
-      <c r="M9" s="44"/>
-      <c r="N9" s="44"/>
-      <c r="O9" s="44"/>
-      <c r="P9" s="45"/>
+      <c r="A9" s="45"/>
+      <c r="B9" s="46"/>
+      <c r="C9" s="46"/>
+      <c r="D9" s="46"/>
+      <c r="E9" s="46"/>
+      <c r="F9" s="46"/>
+      <c r="G9" s="46"/>
+      <c r="H9" s="46"/>
+      <c r="I9" s="46"/>
+      <c r="J9" s="46"/>
+      <c r="K9" s="46"/>
+      <c r="L9" s="46"/>
+      <c r="M9" s="46"/>
+      <c r="N9" s="46"/>
+      <c r="O9" s="46"/>
+      <c r="P9" s="47"/>
     </row>
     <row r="10" spans="1:16" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="24" t="s">
@@ -1045,18 +1062,18 @@
       <c r="P11" s="15"/>
     </row>
     <row r="12" spans="1:16" ht="12" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="46" t="s">
+      <c r="A12" s="39" t="s">
         <v>5</v>
       </c>
       <c r="B12" s="32"/>
       <c r="C12" s="21"/>
       <c r="D12" s="21"/>
-      <c r="E12" s="47"/>
+      <c r="E12" s="40"/>
       <c r="F12" s="21"/>
       <c r="G12" s="22"/>
       <c r="H12" s="23"/>
-      <c r="I12" s="48"/>
-      <c r="J12" s="48"/>
+      <c r="I12" s="41"/>
+      <c r="J12" s="21"/>
       <c r="K12" s="21"/>
       <c r="L12" s="21"/>
       <c r="M12" s="21"/>
@@ -1064,11 +1081,301 @@
       <c r="O12" s="21"/>
       <c r="P12" s="22"/>
     </row>
+    <row r="13" spans="1:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="14" spans="1:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A14" s="4"/>
+      <c r="B14" s="42" t="s">
+        <v>2</v>
+      </c>
+      <c r="C14" s="43"/>
+      <c r="D14" s="43"/>
+      <c r="E14" s="43"/>
+      <c r="F14" s="43"/>
+      <c r="G14" s="44"/>
+      <c r="H14" s="2"/>
+      <c r="I14" s="42" t="s">
+        <v>3</v>
+      </c>
+      <c r="J14" s="43"/>
+      <c r="K14" s="43"/>
+      <c r="L14" s="43"/>
+      <c r="M14" s="43"/>
+      <c r="N14" s="43"/>
+      <c r="O14" s="43"/>
+      <c r="P14" s="44"/>
+    </row>
+    <row r="15" spans="1:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A15" s="5"/>
+      <c r="B15" s="27">
+        <v>1</v>
+      </c>
+      <c r="C15" s="28">
+        <v>2</v>
+      </c>
+      <c r="D15" s="28">
+        <v>3</v>
+      </c>
+      <c r="E15" s="29">
+        <v>4</v>
+      </c>
+      <c r="F15" s="28">
+        <v>5</v>
+      </c>
+      <c r="G15" s="30">
+        <v>6</v>
+      </c>
+      <c r="H15" s="31"/>
+      <c r="I15" s="27">
+        <v>1</v>
+      </c>
+      <c r="J15" s="28">
+        <v>2</v>
+      </c>
+      <c r="K15" s="28">
+        <v>3</v>
+      </c>
+      <c r="L15" s="28">
+        <v>4</v>
+      </c>
+      <c r="M15" s="28">
+        <v>5</v>
+      </c>
+      <c r="N15" s="28">
+        <v>6</v>
+      </c>
+      <c r="O15" s="30">
+        <v>7</v>
+      </c>
+      <c r="P15" s="48">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="16" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A16" s="24" t="s">
+        <v>0</v>
+      </c>
+      <c r="B16" s="1"/>
+      <c r="C16" s="6"/>
+      <c r="D16" s="6"/>
+      <c r="E16" s="7"/>
+      <c r="F16" s="6"/>
+      <c r="G16" s="8"/>
+      <c r="H16" s="9"/>
+      <c r="I16" s="1"/>
+      <c r="J16" s="6"/>
+      <c r="K16" s="6"/>
+      <c r="L16" s="6"/>
+      <c r="M16" s="6"/>
+      <c r="N16" s="10"/>
+      <c r="O16" s="11"/>
+      <c r="P16" s="49"/>
+    </row>
+    <row r="17" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A17" s="25" t="s">
+        <v>11</v>
+      </c>
+      <c r="B17" s="12"/>
+      <c r="C17" s="13"/>
+      <c r="D17" s="13"/>
+      <c r="E17" s="14"/>
+      <c r="F17" s="13"/>
+      <c r="G17" s="15"/>
+      <c r="H17" s="16"/>
+      <c r="I17" s="12"/>
+      <c r="J17" s="13"/>
+      <c r="K17" s="13"/>
+      <c r="L17" s="13"/>
+      <c r="M17" s="17" t="s">
+        <v>1</v>
+      </c>
+      <c r="N17" s="13"/>
+      <c r="O17" s="15"/>
+      <c r="P17" s="50"/>
+    </row>
+    <row r="18" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A18" s="26" t="s">
+        <v>8</v>
+      </c>
+      <c r="B18" s="3"/>
+      <c r="C18" s="18"/>
+      <c r="D18" s="18"/>
+      <c r="E18" s="19"/>
+      <c r="F18" s="18"/>
+      <c r="G18" s="20"/>
+      <c r="H18" s="16"/>
+      <c r="I18" s="3"/>
+      <c r="J18" s="18"/>
+      <c r="K18" s="18"/>
+      <c r="L18" s="17" t="s">
+        <v>1</v>
+      </c>
+      <c r="M18" s="18"/>
+      <c r="N18" s="18"/>
+      <c r="O18" s="20"/>
+      <c r="P18" s="51"/>
+    </row>
+    <row r="19" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A19" s="25" t="s">
+        <v>9</v>
+      </c>
+      <c r="B19" s="12"/>
+      <c r="C19" s="13"/>
+      <c r="D19" s="13"/>
+      <c r="E19" s="14"/>
+      <c r="F19" s="13"/>
+      <c r="G19" s="15"/>
+      <c r="H19" s="16"/>
+      <c r="I19" s="12"/>
+      <c r="J19" s="13"/>
+      <c r="K19" s="17" t="s">
+        <v>1</v>
+      </c>
+      <c r="L19" s="13"/>
+      <c r="M19" s="13"/>
+      <c r="N19" s="13"/>
+      <c r="O19" s="15"/>
+      <c r="P19" s="50"/>
+    </row>
+    <row r="20" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A20" s="26" t="s">
+        <v>6</v>
+      </c>
+      <c r="B20" s="3"/>
+      <c r="C20" s="18"/>
+      <c r="D20" s="18"/>
+      <c r="E20" s="19"/>
+      <c r="F20" s="18"/>
+      <c r="G20" s="20"/>
+      <c r="H20" s="16"/>
+      <c r="I20" s="52"/>
+      <c r="J20" s="17" t="s">
+        <v>1</v>
+      </c>
+      <c r="K20" s="18"/>
+      <c r="L20" s="18"/>
+      <c r="M20" s="18"/>
+      <c r="N20" s="18"/>
+      <c r="O20" s="20"/>
+      <c r="P20" s="51"/>
+    </row>
+    <row r="21" spans="1:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A21" s="38" t="s">
+        <v>4</v>
+      </c>
+      <c r="B21" s="33"/>
+      <c r="C21" s="34"/>
+      <c r="D21" s="34"/>
+      <c r="E21" s="35"/>
+      <c r="F21" s="34"/>
+      <c r="G21" s="36"/>
+      <c r="H21" s="23"/>
+      <c r="I21" s="37" t="s">
+        <v>1</v>
+      </c>
+      <c r="J21" s="34"/>
+      <c r="K21" s="34"/>
+      <c r="L21" s="34"/>
+      <c r="M21" s="34"/>
+      <c r="N21" s="34"/>
+      <c r="O21" s="36"/>
+      <c r="P21" s="50"/>
+    </row>
+    <row r="22" spans="1:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A22" s="45"/>
+      <c r="B22" s="46"/>
+      <c r="C22" s="46"/>
+      <c r="D22" s="46"/>
+      <c r="E22" s="46"/>
+      <c r="F22" s="46"/>
+      <c r="G22" s="46"/>
+      <c r="H22" s="46"/>
+      <c r="I22" s="46"/>
+      <c r="J22" s="46"/>
+      <c r="K22" s="46"/>
+      <c r="L22" s="46"/>
+      <c r="M22" s="46"/>
+      <c r="N22" s="46"/>
+      <c r="O22" s="46"/>
+      <c r="P22" s="47"/>
+    </row>
+    <row r="23" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A23" s="24" t="s">
+        <v>7</v>
+      </c>
+      <c r="B23" s="1"/>
+      <c r="C23" s="6"/>
+      <c r="D23" s="6"/>
+      <c r="E23" s="10" t="s">
+        <v>1</v>
+      </c>
+      <c r="F23" s="10" t="s">
+        <v>1</v>
+      </c>
+      <c r="G23" s="11" t="s">
+        <v>1</v>
+      </c>
+      <c r="H23" s="9"/>
+      <c r="I23" s="1"/>
+      <c r="J23" s="6"/>
+      <c r="K23" s="6"/>
+      <c r="L23" s="6"/>
+      <c r="M23" s="6"/>
+      <c r="N23" s="6"/>
+      <c r="O23" s="6"/>
+      <c r="P23" s="8"/>
+    </row>
+    <row r="24" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A24" s="25" t="s">
+        <v>10</v>
+      </c>
+      <c r="B24" s="12"/>
+      <c r="C24" s="17" t="s">
+        <v>1</v>
+      </c>
+      <c r="D24" s="17" t="s">
+        <v>1</v>
+      </c>
+      <c r="E24" s="14"/>
+      <c r="F24" s="14"/>
+      <c r="G24" s="15"/>
+      <c r="H24" s="16"/>
+      <c r="I24" s="12"/>
+      <c r="J24" s="13"/>
+      <c r="K24" s="13"/>
+      <c r="L24" s="13"/>
+      <c r="M24" s="13"/>
+      <c r="N24" s="13"/>
+      <c r="O24" s="13"/>
+      <c r="P24" s="15"/>
+    </row>
+    <row r="25" spans="1:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A25" s="39" t="s">
+        <v>5</v>
+      </c>
+      <c r="B25" s="32"/>
+      <c r="C25" s="21"/>
+      <c r="D25" s="21"/>
+      <c r="E25" s="40"/>
+      <c r="F25" s="21"/>
+      <c r="G25" s="22"/>
+      <c r="H25" s="23"/>
+      <c r="I25" s="41"/>
+      <c r="J25" s="21"/>
+      <c r="K25" s="21"/>
+      <c r="L25" s="21"/>
+      <c r="M25" s="21"/>
+      <c r="N25" s="21"/>
+      <c r="O25" s="21"/>
+      <c r="P25" s="22"/>
+    </row>
   </sheetData>
-  <mergeCells count="3">
+  <mergeCells count="6">
+    <mergeCell ref="A22:P22"/>
     <mergeCell ref="B1:G1"/>
     <mergeCell ref="I1:P1"/>
     <mergeCell ref="A9:P9"/>
+    <mergeCell ref="B14:G14"/>
+    <mergeCell ref="I14:P14"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>

</xml_diff>